<commit_message>
New UI template added
</commit_message>
<xml_diff>
--- a/Inclusion_sports/Uploads/Tobacco_heterosexsual.xlsx
+++ b/Inclusion_sports/Uploads/Tobacco_heterosexsual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\source\repos\Abhishek10283195\Inclusion_sports\Inclusion_sports\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{76E25004-C814-4DB9-8E77-B8CC8B6234A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E48BB765-9B29-44D7-9328-29A17D13794D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>